<commit_message>
update mô hình csdl
</commit_message>
<xml_diff>
--- a/Mo hinh csdl.xlsx
+++ b/Mo hinh csdl.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Git\Do An web 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Git\Do An web 2\Website---u-gi-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{343ABBFC-5DF3-4AB4-A8C8-74F505E9442E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9C93B4-D4D4-4018-81CF-2E501EDCF3D8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7545" xr2:uid="{CDEF7EE9-4CB3-40D5-B2DE-9F03EA487087}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="66">
   <si>
     <t>Sản phẩm</t>
   </si>
@@ -180,9 +180,6 @@
     <t>Mã ng yêu cầu</t>
   </si>
   <si>
-    <t>Thời gian xin</t>
-  </si>
-  <si>
     <t>Được duyệt hay ko</t>
   </si>
   <si>
@@ -196,6 +193,36 @@
   </si>
   <si>
     <t>Giá max</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>int, A.I</t>
+  </si>
+  <si>
+    <t>nvarchar(200)</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
+    <t>Thời gian người dùng xin</t>
+  </si>
+  <si>
+    <t>nchar(5) {yes,no}</t>
+  </si>
+  <si>
+    <t>nvarchar(1500)</t>
+  </si>
+  <si>
+    <t>nchar(5) {mua, bán, quản trị}</t>
   </si>
 </sst>
 </file>
@@ -217,7 +244,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -227,6 +254,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -243,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -255,6 +288,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
@@ -572,29 +608,31 @@
   <dimension ref="A1:Z25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U4" sqref="U4"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="4" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
     <col min="7" max="7" width="22.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="26.85546875" customWidth="1"/>
     <col min="9" max="9" width="23.140625" customWidth="1"/>
     <col min="10" max="10" width="12.85546875" customWidth="1"/>
     <col min="11" max="11" width="22" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" customWidth="1"/>
     <col min="13" max="13" width="24.5703125" customWidth="1"/>
     <col min="14" max="14" width="11.42578125" customWidth="1"/>
     <col min="15" max="15" width="12.85546875" customWidth="1"/>
     <col min="16" max="16" width="11.7109375" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" customWidth="1"/>
-    <col min="18" max="18" width="11.85546875" customWidth="1"/>
-    <col min="19" max="19" width="18.28515625" customWidth="1"/>
-    <col min="20" max="20" width="14.28515625" customWidth="1"/>
+    <col min="17" max="17" width="14.5703125" customWidth="1"/>
+    <col min="18" max="18" width="19.5703125" customWidth="1"/>
+    <col min="19" max="19" width="23.7109375" customWidth="1"/>
+    <col min="20" max="20" width="17.7109375" customWidth="1"/>
     <col min="21" max="21" width="19.85546875" customWidth="1"/>
     <col min="22" max="22" width="14.140625" customWidth="1"/>
   </cols>
@@ -661,7 +699,7 @@
         <v>19</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V1" s="3" t="s">
         <v>19</v>
@@ -672,128 +710,182 @@
       <c r="Z1" s="3"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="F2" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="G2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
+      <c r="H2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="1"/>
+      <c r="J2" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="K2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1" t="s">
+      <c r="L2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="1"/>
+      <c r="N2" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="O2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1" t="s">
+      <c r="P2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="R2" s="1"/>
+      <c r="R2" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="S2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1" t="s">
+      <c r="T2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="U2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="V2" s="1"/>
+      <c r="V2" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="G3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1" t="s">
+      <c r="H3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="1"/>
+      <c r="J3" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="K3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1" t="s">
+      <c r="L3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="N3" s="1"/>
+      <c r="N3" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="O3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1" t="s">
+      <c r="P3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q3" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="R3" s="1"/>
+      <c r="R3" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="S3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="V3" s="1"/>
+      <c r="T3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1" t="s">
+      <c r="D4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="F4" s="5" t="s">
+        <v>61</v>
+      </c>
       <c r="G4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L4" s="1"/>
+      <c r="L4" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
@@ -801,33 +893,43 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="V4" s="1"/>
+        <v>62</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="U4" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="V4" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="G5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -839,9 +941,11 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="T5" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
@@ -850,10 +954,12 @@
       <c r="Z5" s="1"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="5" t="s">
+        <v>61</v>
+      </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -861,7 +967,9 @@
       <c r="G6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -882,10 +990,12 @@
       <c r="Z6" s="1"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="5" t="s">
+        <v>61</v>
+      </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -893,7 +1003,9 @@
       <c r="G7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="1"/>
+      <c r="H7" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -914,10 +1026,12 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -925,7 +1039,9 @@
       <c r="G8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -946,10 +1062,12 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -957,7 +1075,9 @@
       <c r="G9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -978,10 +1098,12 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -989,7 +1111,9 @@
       <c r="G10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -1010,18 +1134,22 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H11" s="1"/>
+        <v>52</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -1042,10 +1170,12 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1072,10 +1202,12 @@
       <c r="Z12" s="1"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1094,10 +1226,12 @@
       <c r="R13" s="1"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="1"/>
+      <c r="B14" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1116,10 +1250,12 @@
       <c r="R14" s="1"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="1"/>
+      <c r="B15" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>

</xml_diff>

<commit_message>
tạo trang ng bán
</commit_message>
<xml_diff>
--- a/Mo hinh csdl.xlsx
+++ b/Mo hinh csdl.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Git\Do An web 2\Website---u-gi-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A77DA5-8461-45E1-8195-1321A6AB655D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE60E74F-C3CB-439F-ACBD-73535FE59C04}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7545" xr2:uid="{CDEF7EE9-4CB3-40D5-B2DE-9F03EA487087}"/>
   </bookViews>
@@ -138,9 +138,6 @@
     <t>Đã được đấu giá xong chưa</t>
   </si>
   <si>
-    <t>Thời gian quyền đăng bán</t>
-  </si>
-  <si>
     <t>Tự động gia hạn</t>
   </si>
   <si>
@@ -223,6 +220,9 @@
   </si>
   <si>
     <t>Thời gian người dùng yêu cầu</t>
+  </si>
+  <si>
+    <t>Quyền đăng bán</t>
   </si>
 </sst>
 </file>
@@ -625,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{294C9A5C-A2AC-4516-98A8-76B21586D426}">
   <dimension ref="A1:Z25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="S5" sqref="S5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,10 +663,10 @@
         <v>19</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>9</v>
@@ -699,25 +699,25 @@
         <v>19</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>19</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R1" s="3" t="s">
         <v>19</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="V1" s="3" t="s">
         <v>19</v>
@@ -732,67 +732,67 @@
         <v>8</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>18</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>11</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K2" s="7" t="s">
         <v>32</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>11</v>
       </c>
       <c r="N2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="R2" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="O2" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>57</v>
-      </c>
       <c r="S2" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="U2" s="6" t="s">
         <v>11</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
@@ -804,67 +804,67 @@
         <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>29</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>11</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M3" s="6" t="s">
         <v>35</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="S3" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="U3" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V3" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
@@ -876,25 +876,25 @@
         <v>16</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -902,7 +902,7 @@
         <v>33</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -911,16 +911,16 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U4" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="V4" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
@@ -932,7 +932,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -940,13 +940,13 @@
         <v>14</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -959,10 +959,10 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
@@ -976,7 +976,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -986,7 +986,7 @@
         <v>24</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -1012,7 +1012,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -1022,7 +1022,7 @@
         <v>25</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -1048,7 +1048,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -1058,7 +1058,7 @@
         <v>26</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -1083,7 +1083,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1093,7 +1093,7 @@
         <v>27</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -1119,14 +1119,14 @@
         <v>6</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>61</v>
@@ -1155,17 +1155,17 @@
         <v>7</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -1191,7 +1191,7 @@
         <v>20</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1223,7 +1223,7 @@
         <v>30</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1247,7 +1247,7 @@
         <v>36</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1268,10 +1268,10 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>

</xml_diff>